<commit_message>
fixed error with loss/profit not displaying in result page after trade closuer
</commit_message>
<xml_diff>
--- a/ForexTrades.xlsx
+++ b/ForexTrades.xlsx
@@ -9,6 +9,10 @@
   <sheets>
     <sheet name="26-5-23 - 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="26-5-23 - 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="26-5-23 - 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="27-5-23 - 1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="27-5-23 - 2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="27-5-23 - 3" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -190,6 +194,123 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10001250" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10001250" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10001250" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>11</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10001250" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -795,4 +916,617 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="150" customWidth="1" min="9" max="9"/>
+    <col width="150" customWidth="1" min="10" max="10"/>
+    <col width="150" customWidth="1" min="11" max="11"/>
+    <col width="150" customWidth="1" min="12" max="12"/>
+    <col hidden="1" outlineLevel="1" width="13" customWidth="1" min="13" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Pair</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lot-size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Buy-sell</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pos-size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Loss-gain</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>4-hour</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>1-hour</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>15-min</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GBP/CAD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1.68124</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.68124</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>£55.33</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>D:/Personal Projects Git/DocKeep/Charts/4.PNG</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>D:/Personal Projects Git/DocKeep/Charts/1.PNG</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>D:/Personal Projects Git/DocKeep/Charts/15.PNG</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>D:/Personal Projects Git/DocKeep/Charts/R.PNG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Notes:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Confluences:</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:G12"/>
+    <mergeCell ref="B15:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="150" customWidth="1" min="9" max="9"/>
+    <col width="150" customWidth="1" min="10" max="10"/>
+    <col width="150" customWidth="1" min="11" max="11"/>
+    <col width="150" customWidth="1" min="12" max="12"/>
+    <col hidden="1" outlineLevel="1" width="13" customWidth="1" min="13" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Pair</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lot-size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Buy-sell</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pos-size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Loss-gain</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>4-hour</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>1-hour</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>15-min</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GBP/CAD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1.68097</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.68097</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>£55.33</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Notes:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Confluences:</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:G12"/>
+    <mergeCell ref="B15:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="150" customWidth="1" min="9" max="9"/>
+    <col width="150" customWidth="1" min="10" max="10"/>
+    <col width="150" customWidth="1" min="11" max="11"/>
+    <col width="150" customWidth="1" min="12" max="12"/>
+    <col hidden="1" outlineLevel="1" width="13" customWidth="1" min="13" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Pair</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lot-size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Buy-sell</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pos-size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Loss-gain</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>4-hour</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>1-hour</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>15-min</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AUD/USD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>£55.33</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>26.36</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Notes:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Confluences:</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:G12"/>
+    <mergeCell ref="B15:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="150" customWidth="1" min="9" max="9"/>
+    <col width="150" customWidth="1" min="10" max="10"/>
+    <col width="150" customWidth="1" min="11" max="11"/>
+    <col width="150" customWidth="1" min="12" max="12"/>
+    <col hidden="1" outlineLevel="1" width="13" customWidth="1" min="13" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Pair</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lot-size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Buy-sell</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pos-size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Loss-gain</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>4-hour</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>1-hour</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>15-min</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GBP/CAD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1.68097</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.68097</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>£55.33</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Notes:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Confluences:</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:G12"/>
+    <mergeCell ref="B15:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
introduced better folder structure
</commit_message>
<xml_diff>
--- a/ForexTrades.xlsx
+++ b/ForexTrades.xlsx
@@ -13,6 +13,7 @@
     <sheet name="27-5-23 - 1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="27-5-23 - 2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="27-5-23 - 3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="28-5-23 - 1" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -311,6 +312,39 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10001250" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1529,4 +1563,158 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="150" customWidth="1" min="9" max="9"/>
+    <col width="150" customWidth="1" min="10" max="10"/>
+    <col width="150" customWidth="1" min="11" max="11"/>
+    <col width="150" customWidth="1" min="12" max="12"/>
+    <col hidden="1" outlineLevel="1" width="13" customWidth="1" min="13" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Pair</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lot-size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Buy-sell</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pos-size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Loss-gain</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>4-hour</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>1-hour</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>15-min</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AUD/USD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.65195</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.65195</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>£55.33</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>26.36</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>D:/Personal Projects Git/DocKeep/Charts/4.PNG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Notes:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Confluences:</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:G12"/>
+    <mergeCell ref="B15:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>